<commit_message>
updated plant health index
</commit_message>
<xml_diff>
--- a/02_output/09_plant_health/phi_mean_total.xlsx
+++ b/02_output/09_plant_health/phi_mean_total.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Root health score</t>
   </si>
   <si>
-    <t xml:space="preserve">Specific Leaf Area (g/cm2)</t>
+    <t xml:space="preserve">SLA (g/cm2)</t>
   </si>
   <si>
     <t xml:space="preserve">Yield (dt/ha)</t>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">phi_total</t>
   </si>
   <si>
-    <t xml:space="preserve">phi_total_without_yield</t>
+    <t xml:space="preserve">phi_total_no_yield</t>
   </si>
   <si>
     <t xml:space="preserve">1_1</t>
@@ -546,10 +546,10 @@
         <v>#NUM!</v>
       </c>
       <c r="I4" t="n">
-        <v>2.58778082264849</v>
+        <v>1.29389041132425</v>
       </c>
       <c r="J4" t="n">
-        <v>2.58778082264849</v>
+        <v>1.29389041132425</v>
       </c>
     </row>
     <row r="5">
@@ -770,10 +770,10 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>1.43083322920571</v>
+        <v>1.35850618518056</v>
       </c>
       <c r="J11" t="n">
-        <v>1.43083322920571</v>
+        <v>1.35850618518056</v>
       </c>
     </row>
     <row r="12">

</xml_diff>